<commit_message>
Align 2018 and 2019 capacity values with historical data
</commit_message>
<xml_diff>
--- a/InputData/elec/SYC/Start Year Capacities.xlsx
+++ b/InputData/elec/SYC/Start Year Capacities.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\Dropbox\EPS\Input Data for India 2.0\elec\SYC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\OneDrive\Desktop\vensim test\Updated power sector data - 20200624\SYC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D825D5B0-5AF5-4794-A1C9-046418823D6A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C640D9-CDEE-4879-B057-B366B6C5788E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
   <si>
     <t>SYC Start Year Electricity Generation Capacity</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Source:</t>
   </si>
   <si>
-    <t>Central Electricity authority</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
     <t>Peaking gas</t>
   </si>
   <si>
-    <t>http://www.cea.nic.in/reports/monthly/installedcapacity/2018/installed_capacity-12.pdf</t>
-  </si>
-  <si>
     <t>Capacity as on 31.12.2018 (MW)</t>
   </si>
   <si>
@@ -160,36 +154,9 @@
     <t>pp 8.5</t>
   </si>
   <si>
-    <t>pp 10.2</t>
-  </si>
-  <si>
-    <t>of the 23075.57 MW of gas based capacity available in 2017, 350 MW is open cycle 
-which is suited for peaking. From 2017-22, 406 MW new gas plants are expected to be installed by NEP.
-These are all combined cycle, or engine-type - which are considered suitable for peaking by NEP 
-(see NEP report excerpts in CEA-Data sheet). We assume that this new capacity is included as per plan in the 2018 
-installed capacity figures, as the current sources for 2018 don't disaggregate the gas power plants by type.
-Dividing the 406 value by 5 and adding it to 2018 could lead to potential double counting, which is a risk considering
-that gas plants are already operating at low PLFs due to shortage of fuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacities by Plant Type </t>
-  </si>
-  <si>
-    <t>December 2018 (Monthly Installed Cap report)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peaking gas </t>
-  </si>
-  <si>
-    <t>Central Electricity Authority - National Electricity Plan Volume 1</t>
-  </si>
-  <si>
     <t>2018</t>
   </si>
   <si>
-    <t>Table 10.3, 10.4, Section 6.10.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">As official data has no detailed breakdown of liquid fuel plants, </t>
   </si>
   <si>
@@ -199,21 +166,9 @@
     <t>Only natural gas open cycle plants are included as peaking plants .</t>
   </si>
   <si>
-    <t>No geothermal, solar thermal, offshore wind or MSW plants were operational/installed in 2018.</t>
-  </si>
-  <si>
-    <t>Waste to energy is accounted under biomass.</t>
-  </si>
-  <si>
     <t>Hydro includes large, small, and pumped storage.</t>
   </si>
   <si>
-    <t>As of March 2019, there is 4786 MW of pumped hydro storage capacity out of which 3305 is working.</t>
-  </si>
-  <si>
-    <t>This is included in large hydro, as the peaker plants are classified only as natural gas in EPS.</t>
-  </si>
-  <si>
     <t>It is assumed that all peaking plants provide flexibility points.</t>
   </si>
   <si>
@@ -233,13 +188,71 @@
   </si>
   <si>
     <t>Diesel is accounted in petroleum subscript of EPS.</t>
+  </si>
+  <si>
+    <t>Pp 8.5</t>
+  </si>
+  <si>
+    <t>However, pumped hydro storage plants are not considered for peaking, as the peaker plants are classified only as natural gas in EPS.</t>
+  </si>
+  <si>
+    <t>Large Hydro Capacity by type</t>
+  </si>
+  <si>
+    <t>Central Electricity Authority</t>
+  </si>
+  <si>
+    <t>Monthly Hydro Reports (archives)</t>
+  </si>
+  <si>
+    <t>Monthly Installed Capacity Reports (archives)</t>
+  </si>
+  <si>
+    <t>Central Electricity Authority - National Electricity Plan (NEP) Volume 1</t>
+  </si>
+  <si>
+    <t>Peaking gas capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installed Capacities by Plant Type </t>
+  </si>
+  <si>
+    <t>Dec 2017</t>
+  </si>
+  <si>
+    <t>Installed Capacity, 2017, Source-wise</t>
+  </si>
+  <si>
+    <t>http://www.cea.nic.in/reports/monthly/installedcapacity/2017/installed_capacity-12.pdf</t>
+  </si>
+  <si>
+    <t>Installed Large Hydro Capacity, 2017, by type</t>
+  </si>
+  <si>
+    <t>http://www.cea.nic.in/reports/monthly/hydro/2017/hydro_stations-12.pdf</t>
+  </si>
+  <si>
+    <t>As of Dec 2017, there is 4786 MW of pumped hydro storage capacity which is included in CEA's reporting of Large Hydro Capacity.</t>
+  </si>
+  <si>
+    <t>Waste to energy is accounted under Municipal Solid Waste.</t>
+  </si>
+  <si>
+    <t>No lignite plants were operational in 2017.</t>
+  </si>
+  <si>
+    <t>No geothermal, solar thermal, offshore wind capacity existed in 2017.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As per CEA's NEP, of the monitored natural gas based capacity in March 2017, 350 MW is open cycle 
+which is suited for peaking. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,13 +296,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -331,7 +337,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -349,10 +355,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -382,23 +384,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>5103</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>166688</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>177892</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>136070</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>225378</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>81483</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4961D332-2CAA-425A-973E-821085AF0C57}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED5E7876-9F37-43F3-B523-1E010767E687}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -414,51 +416,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="761999" y="0"/>
-          <a:ext cx="10083893" cy="8518070"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>136072</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>356347</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>10045</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED5E7876-9F37-43F3-B523-1E010767E687}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10804072" y="5810250"/>
+          <a:off x="11435103" y="166688"/>
           <a:ext cx="8602275" cy="3724795"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -470,15 +428,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>35719</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>153591</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>189310</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>47924</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -495,14 +453,14 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10668000" y="10477500"/>
+          <a:off x="11465719" y="4572000"/>
           <a:ext cx="8535591" cy="2143424"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -514,23 +472,67 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>612322</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>27213</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>43637</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>348914</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
+        <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C90F85A0-A1C5-4FD9-A5BD-8C952C42E8B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CA6094A-B9E8-44C5-AB50-C1CB4A4F3921}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="761999" y="0"/>
+          <a:ext cx="9492915" cy="6858000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>420435</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>133581</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42637201-6E01-4BAF-B893-64AB0E35726D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -546,8 +548,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11280322" y="0"/>
-          <a:ext cx="6272891" cy="4425137"/>
+          <a:off x="762000" y="7048500"/>
+          <a:ext cx="9564435" cy="1657581"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>91329</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>188004</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25A98D3A-04E0-4763-B224-C9D41EF749EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762001" y="9235329"/>
+          <a:ext cx="6810374" cy="4478175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -822,15 +868,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:D23"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="100.28515625" customWidth="1"/>
+    <col min="4" max="4" width="68.5703125" customWidth="1"/>
     <col min="8" max="8" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -849,124 +896,148 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>58</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>49</v>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A23:D23"/>
-  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{A7FD3E81-E6F0-4C52-ACE1-F41AA516BB92}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{99545776-ED11-4F9A-9C9F-F032AC795A24}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{153D1619-2DEF-4C19-B7AF-A3ED3991C636}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -980,7 +1051,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,15 +1062,15 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="11">
-        <v>191092.5</v>
+        <v>192971.5</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
@@ -1010,23 +1081,23 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="11">
-        <v>24937.22</v>
+        <v>25150.38</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="11">
-        <v>637.63</v>
+        <v>837.63</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="11">
         <v>6780</v>
@@ -1034,59 +1105,59 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="11">
-        <v>45399.22</v>
+        <v>44963.42</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="11">
-        <v>4517.45</v>
+        <v>4418.1499999999996</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="11">
-        <v>35138.15</v>
+        <v>32848.46</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="11">
-        <v>9075.5</v>
+        <v>8413.7999999999993</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="11">
-        <v>138.30000000000001</v>
+        <v>114.08</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="11">
-        <v>25212.26</v>
+        <v>17052.41</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13">
         <f>SUM(C2:C11)</f>
-        <v>342928.23000000004</v>
+        <v>333549.83</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1094,16 +1165,16 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="11">
-        <v>6360</v>
+        <v>0</v>
       </c>
       <c r="D15" s="3"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17">
         <v>350</v>
@@ -1122,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B21:P69"/>
+  <dimension ref="B21:P74"/>
   <sheetViews>
-    <sheetView topLeftCell="C25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,45 +1204,54 @@
     <row r="21" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O21" s="3"/>
     </row>
-    <row r="26" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="P26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="P27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="3" t="s">
+    <row r="22" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="P22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O52" t="s">
+    <row r="23" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="P23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P37" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O53" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="68" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O68" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="69" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O69" t="s">
-        <v>38</v>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B48" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B48" r:id="rId1" xr:uid="{DF86306B-D430-4107-A4C2-306995175FA7}"/>
+    <hyperlink ref="B74" r:id="rId2" xr:uid="{1A0036FD-787C-49C9-81C1-AC9881804B7B}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1188,7 +1268,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,25 +1280,25 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="6">
         <f>Calcs!C2</f>
-        <v>191092.5</v>
+        <v>192971.5</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1229,11 +1309,11 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="6">
         <f>Calcs!C3-Calcs!C17</f>
-        <v>24587.22</v>
+        <v>24800.38</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1244,7 +1324,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="6">
         <f>Calcs!C5</f>
@@ -1259,11 +1339,11 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="6">
         <f>Calcs!C6+Calcs!C7</f>
-        <v>49916.67</v>
+        <v>49381.57</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1274,11 +1354,11 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="6">
         <f>Calcs!C8</f>
-        <v>35138.15</v>
+        <v>32848.46</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1289,11 +1369,11 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="6">
         <f>Calcs!C11</f>
-        <v>25212.26</v>
+        <v>17052.41</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1304,7 +1384,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="6">
         <v>0</v>
@@ -1318,11 +1398,11 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="6">
         <f>Calcs!C9</f>
-        <v>9075.5</v>
+        <v>8413.7999999999993</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1333,7 +1413,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="6">
         <f>0</f>
@@ -1348,11 +1428,11 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="6">
         <f>Calcs!C4</f>
-        <v>637.63</v>
+        <v>837.63</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1363,7 +1443,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="6">
         <f>Calcs!C17</f>
@@ -1378,11 +1458,11 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="6">
         <f>Calcs!C15</f>
-        <v>6360</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1393,7 +1473,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="6">
         <f>0</f>
@@ -1408,7 +1488,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1422,7 +1502,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1436,11 +1516,11 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B17" s="6">
         <f>Calcs!C10</f>
-        <v>138.30000000000001</v>
+        <v>114.08</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1479,14 +1559,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="7">
         <v>1</v>

</xml_diff>